<commit_message>
Changed alignment of some things.
</commit_message>
<xml_diff>
--- a/teamContributions.xlsx
+++ b/teamContributions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/22356053_studentmail_ul_ie/Documents/Year 2/CS4013 - Object Orientated Development/UL-Student-Record-System/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{E33900B6-0768-43BB-ACDD-D2B520B8A2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAB5C396-9461-4EA3-B165-402411175EF7}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{E33900B6-0768-43BB-ACDD-D2B520B8A2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2899141-17A2-4AE8-A88E-A74A899659BE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -256,16 +256,18 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -282,6 +284,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -583,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,24 +604,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1049,13 +1055,13 @@
       <c r="A34" s="9">
         <v>45241</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F34" s="3"/>
@@ -1064,13 +1070,13 @@
       <c r="A35" s="9">
         <v>45242</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F35" s="3"/>
@@ -1079,13 +1085,13 @@
       <c r="A36" s="9">
         <v>45244</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F36" s="3"/>
@@ -1094,13 +1100,13 @@
       <c r="A37" s="9">
         <v>45245</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F37" s="3"/>
@@ -1109,13 +1115,13 @@
       <c r="A38" s="9">
         <v>45249</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F38" s="3"/>
@@ -1124,13 +1130,13 @@
       <c r="A39" s="9">
         <v>45250</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F39" s="3"/>
@@ -1139,13 +1145,13 @@
       <c r="A40" s="9">
         <v>45252</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F40" s="3"/>
@@ -1154,13 +1160,13 @@
       <c r="A41" s="9">
         <v>45255</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F41" s="3"/>
@@ -1169,13 +1175,13 @@
       <c r="A42" s="9">
         <v>45257</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="3"/>

</xml_diff>

<commit_message>
updated HelpFile.pdf and teamContributions.xlsx
</commit_message>
<xml_diff>
--- a/teamContributions.xlsx
+++ b/teamContributions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/22356053_studentmail_ul_ie/Documents/Year 2/CS4013 - Object Orientated Development/UL-Student-Record-System/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LM174\CS4013\UL-Student-Record-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{E33900B6-0768-43BB-ACDD-D2B520B8A2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2899141-17A2-4AE8-A88E-A74A899659BE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBA219B-1509-4462-9DD3-BA5850EB4323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -259,14 +259,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -284,10 +284,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -590,7 +586,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,24 +600,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="C2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -895,7 +891,10 @@
         <v>29</v>
       </c>
       <c r="C21" s="3">
-        <v>1</v>
+        <v>0.95</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.05</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="1"/>
@@ -1052,7 +1051,7 @@
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="9">
+      <c r="A34" s="7">
         <v>45241</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -1067,7 +1066,7 @@
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="9">
+      <c r="A35" s="7">
         <v>45242</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -1082,7 +1081,7 @@
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="9">
+      <c r="A36" s="7">
         <v>45244</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -1097,7 +1096,7 @@
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="9">
+      <c r="A37" s="7">
         <v>45245</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -1112,7 +1111,7 @@
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="9">
+      <c r="A38" s="7">
         <v>45249</v>
       </c>
       <c r="B38" s="6" t="s">
@@ -1127,7 +1126,7 @@
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="9">
+      <c r="A39" s="7">
         <v>45250</v>
       </c>
       <c r="B39" s="6" t="s">
@@ -1142,7 +1141,7 @@
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="9">
+      <c r="A40" s="7">
         <v>45252</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -1157,7 +1156,7 @@
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="9">
+      <c r="A41" s="7">
         <v>45255</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -1172,7 +1171,7 @@
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="9">
+      <c r="A42" s="7">
         <v>45257</v>
       </c>
       <c r="B42" s="6" t="s">

</xml_diff>